<commit_message>
Added code and updated HESS
</commit_message>
<xml_diff>
--- a/HESS/Amparo.xlsx
+++ b/HESS/Amparo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natashasekhon/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF7C1C3A-4E78-D647-B905-F19366FA2217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E8BD8F6-0FD3-7642-8E38-67D384F8EA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15940" xr2:uid="{1177C2E8-E44D-7046-AA7C-1A347536FC2F}"/>
+    <workbookView xWindow="12600" yWindow="1000" windowWidth="15820" windowHeight="16440" xr2:uid="{DBBC2395-E4E2-104E-9132-01771B5AA88E}"/>
   </bookViews>
   <sheets>
     <sheet name="AMPARO" sheetId="1" r:id="rId1"/>
@@ -1272,7 +1272,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABA3786D-C11A-C24D-9ED7-5C98D52B8CC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B94FD9E-A1F7-BB41-B8B1-4C08E3856448}">
   <dimension ref="A1:O281"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">

</xml_diff>